<commit_message>
11, 14, 8, 9
</commit_message>
<xml_diff>
--- a/8/8.xlsx
+++ b/8/8.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -9,9 +9,8 @@
   <sheets>
     <sheet name="7" sheetId="2" r:id="rId1"/>
     <sheet name="8" sheetId="1" r:id="rId2"/>
-    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -48,8 +47,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,24 +231,13 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -424,159 +412,158 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>1.8779868730901299</c:v>
+                  <c:v>2.1872365302278198</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.04872358151307</c:v>
+                  <c:v>0.76846818474802903</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.11327510203060701</c:v>
+                  <c:v>0.12998580019261799</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.970365400648735</c:v>
+                  <c:v>-0.61072598466451999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.5357634841038601</c:v>
+                  <c:v>-2.0551884125620599</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-3.55584228067538</c:v>
+                  <c:v>-3.2058232097278601</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-3.9474333387310598</c:v>
+                  <c:v>-3.6322381336357701</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-5.2650230324766403</c:v>
+                  <c:v>-4.7736779123442004</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-5.6800610199923502</c:v>
+                  <c:v>-6.0343239617040396</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-7.1697105405861201</c:v>
+                  <c:v>-6.8664907019936399</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-8.4510175509625007</c:v>
+                  <c:v>-8.5173925622634901</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-9.2922791804804898</c:v>
+                  <c:v>-9.0479142547529108</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-9.9736265496153393</c:v>
+                  <c:v>-10.0479453771409</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-11.554235043452</c:v>
+                  <c:v>-10.850570603016999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-12.1472185351737</c:v>
+                  <c:v>-12.0362376775436</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-13.1447956249076</c:v>
+                  <c:v>-12.7598399255463</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-13.7740670272578</c:v>
+                  <c:v>-14.1339499801439</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-15.021928223002799</c:v>
+                  <c:v>-14.705421269934799</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-15.9907308170609</c:v>
+                  <c:v>-16.325043785474499</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-17.178151585884802</c:v>
+                  <c:v>-17.149970099539999</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-18.6823021269769</c:v>
+                  <c:v>-17.932165894331799</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-18.808398949611799</c:v>
+                  <c:v>-19.0326634461819</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-19.669055903805202</c:v>
+                  <c:v>-19.939167397070101</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-20.441670629015501</c:v>
+                  <c:v>-20.779483445282001</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-22.079246939808399</c:v>
+                  <c:v>-22.745912509466699</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-23.2016704762394</c:v>
+                  <c:v>27.620864522782998</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-24.161095070809701</c:v>
+                  <c:v>-23.7800308439706</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-24.8766582272454</c:v>
+                  <c:v>-25.331097463237398</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-26.0737989722431</c:v>
+                  <c:v>-26.1627850994984</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-26.8424819664715</c:v>
+                  <c:v>-26.734834108011</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-27.646865616063</c:v>
+                  <c:v>-28.003024083911299</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-28.802772837058999</c:v>
+                  <c:v>-28.810774424788701</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-29.811864889133499</c:v>
+                  <c:v>-30.255902003966298</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-30.819992693750301</c:v>
+                  <c:v>-30.796419406734699</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-32.047658828927297</c:v>
+                  <c:v>-31.7479428462368</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-33.6739143451302</c:v>
+                  <c:v>-32.715962063456402</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-33.887727907480901</c:v>
+                  <c:v>-33.788552156288702</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-34.772603885398603</c:v>
+                  <c:v>-35.3104929373755</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-36.140216914653102</c:v>
+                  <c:v>-35.793556789608402</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-37.127676445117302</c:v>
+                  <c:v>-37.551172608759998</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>-37.357523155733901</c:v>
+                  <c:v>-38.233033222547199</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>-38.412719576328598</c:v>
+                  <c:v>-39.0356740179909</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>-40.113887699237203</c:v>
+                  <c:v>-40.3164542089959</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-41.318860316085697</c:v>
+                  <c:v>-41.412564372814401</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>-42.261308051520302</c:v>
+                  <c:v>-41.805156520057999</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-43.136103750477503</c:v>
+                  <c:v>-42.836516776315001</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>-44.212076715397799</c:v>
+                  <c:v>-44.089090134612803</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>-45.061877624970499</c:v>
+                  <c:v>-44.694716291171602</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>-46.283588040614902</c:v>
+                  <c:v>-45.795324866667102</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-47.205619537623299</c:v>
+                  <c:v>2.81341692842153</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -753,199 +740,186 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>1.9729970999999999</c:v>
+                  <c:v>2.0357048</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.97275376999999996</c:v>
+                  <c:v>1.0347188</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.7489560000000024E-2</c:v>
+                  <c:v>3.3732800000000118E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.02773289</c:v>
+                  <c:v>-0.96725319999999959</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-2.0279762200000002</c:v>
+                  <c:v>-1.9682391999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-3.0282195500000002</c:v>
+                  <c:v>-2.9692251999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-4.0284628800000002</c:v>
+                  <c:v>-3.9702111999999992</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-5.0287062100000002</c:v>
+                  <c:v>-4.9711971999999989</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-6.0289495400000002</c:v>
+                  <c:v>-5.9721831999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-7.0291928700000001</c:v>
+                  <c:v>-6.9731691999999992</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-8.0294361999999992</c:v>
+                  <c:v>-7.9741552000000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-9.0296795299999992</c:v>
+                  <c:v>-8.9751411999999995</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-10.029922859999999</c:v>
+                  <c:v>-9.9761271999999988</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-11.030166189999999</c:v>
+                  <c:v>-10.9771132</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-12.030409519999999</c:v>
+                  <c:v>-11.978099199999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-13.030652849999999</c:v>
+                  <c:v>-12.9790852</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-14.030896179999999</c:v>
+                  <c:v>-13.980071199999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-15.031139509999999</c:v>
+                  <c:v>-14.9810572</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-16.031382839999999</c:v>
+                  <c:v>-15.982043199999998</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-17.031626169999999</c:v>
+                  <c:v>-16.983029199999997</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-18.031869499999999</c:v>
+                  <c:v>-17.984015199999998</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-19.032112829999999</c:v>
+                  <c:v>-18.985001199999996</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-20.032356159999999</c:v>
+                  <c:v>-19.985987199999997</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-21.032599489999999</c:v>
+                  <c:v>-20.986973199999998</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-22.032842819999999</c:v>
+                  <c:v>-21.987959199999995</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-23.033086149999999</c:v>
+                  <c:v>-22.988945199999996</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-24.033329479999999</c:v>
+                  <c:v>-23.989931199999997</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-25.033572809999999</c:v>
+                  <c:v>-24.990917199999998</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-26.033816139999999</c:v>
+                  <c:v>-25.991903199999996</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-27.034059469999999</c:v>
+                  <c:v>-26.992889199999997</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-28.034302799999999</c:v>
+                  <c:v>-27.993875199999998</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-29.034546129999999</c:v>
+                  <c:v>-28.994861199999995</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-30.034789459999999</c:v>
+                  <c:v>-29.995847199999996</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-31.035032790000002</c:v>
+                  <c:v>-30.996833199999994</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-32.035276119999999</c:v>
+                  <c:v>-31.997819199999999</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-33.035519449999995</c:v>
+                  <c:v>-32.9988052</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-34.035762779999999</c:v>
+                  <c:v>-33.999791199999997</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-35.036006110000002</c:v>
+                  <c:v>-35.000777200000002</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-36.036249439999999</c:v>
+                  <c:v>-36.001763199999999</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-37.036492769999995</c:v>
+                  <c:v>-37.002749199999997</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>-38.036736099999999</c:v>
+                  <c:v>-38.003735200000001</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>-39.036979430000002</c:v>
+                  <c:v>-39.004721199999999</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>-40.037222759999999</c:v>
+                  <c:v>-40.005707199999996</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-41.037466089999995</c:v>
+                  <c:v>-41.006693200000001</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>-42.037709419999999</c:v>
+                  <c:v>-42.007679199999998</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-43.037952750000002</c:v>
+                  <c:v>-43.008665199999996</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>-44.038196079999999</c:v>
+                  <c:v>-44.0096512</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>-45.038439409999995</c:v>
+                  <c:v>-45.010637199999998</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>-46.038682739999999</c:v>
+                  <c:v>-46.011623199999995</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-47.038926070000002</c:v>
+                  <c:v>-47.0126092</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="293550272"/>
-        <c:axId val="293551424"/>
+        <c:axId val="160224768"/>
+        <c:axId val="160226304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="293550272"/>
+        <c:axId val="160224768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="293551424"/>
+        <c:crossAx val="160226304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="293551424"/>
+        <c:axId val="160226304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="293550272"/>
+        <c:crossAx val="160224768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -953,15 +927,13 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -969,24 +941,13 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1161,159 +1122,158 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>11.0476492914418</c:v>
+                  <c:v>10.804663868816901</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.2545142953972</c:v>
+                  <c:v>11.4045971550992</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.0478921072727</c:v>
+                  <c:v>12.313315363637299</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.6540812020831</c:v>
+                  <c:v>12.184555948423499</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.890539310361</c:v>
+                  <c:v>12.7327705178178</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.0601016876484</c:v>
+                  <c:v>13.389541335015201</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.8883663155998</c:v>
+                  <c:v>13.7616845144299</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14.352919110137501</c:v>
+                  <c:v>14.6842531129822</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15.023211056700401</c:v>
+                  <c:v>15.114017126027999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15.5941525930727</c:v>
+                  <c:v>15.3782795925491</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15.984676567108201</c:v>
+                  <c:v>16.381627265468101</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16.990543270915001</c:v>
+                  <c:v>16.3852456138709</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>17.401500291947201</c:v>
+                  <c:v>17.070852956278099</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>17.5194324450365</c:v>
+                  <c:v>16.898206296146999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>18.3529038861057</c:v>
+                  <c:v>17.738664734695401</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>18.660639069482599</c:v>
+                  <c:v>18.675725948944301</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>18.6534590387535</c:v>
+                  <c:v>19.291096258252701</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>19.520696531085001</c:v>
+                  <c:v>19.6516583360029</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>20.257854904623802</c:v>
+                  <c:v>20.069991577437701</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20.506458991237299</c:v>
+                  <c:v>20.527395543142202</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>21.2606427062012</c:v>
+                  <c:v>20.8450971527189</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21.598616288808199</c:v>
+                  <c:v>21.541101164524498</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>21.942345412099101</c:v>
+                  <c:v>21.866320369385001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>22.496036689624599</c:v>
+                  <c:v>22.355525151997401</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>22.686528292361</c:v>
+                  <c:v>22.848657320085199</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>23.852812302278299</c:v>
+                  <c:v>-26.525142054605301</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>23.694499773141999</c:v>
+                  <c:v>23.615863345663801</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>24.7768002538944</c:v>
+                  <c:v>24.231967601597901</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>24.654619350632998</c:v>
+                  <c:v>25.1513006226442</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>25.4495145582415</c:v>
+                  <c:v>25.1571646801257</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>25.671706507480401</c:v>
+                  <c:v>25.777402875439702</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>26.440430508471</c:v>
+                  <c:v>26.264182636778699</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>26.939591096962101</c:v>
+                  <c:v>26.884713652702501</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>27.662355371868099</c:v>
+                  <c:v>27.110427364873299</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>27.7275294876614</c:v>
+                  <c:v>28.432701226955999</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>28.2897176785849</c:v>
+                  <c:v>28.544306139202899</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>29.012454496925098</c:v>
+                  <c:v>29.160002278887799</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>29.658489995003102</c:v>
+                  <c:v>29.578328888553099</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>30.185380841339601</c:v>
+                  <c:v>29.926789950360298</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>30.475054220399802</c:v>
+                  <c:v>30.624062254067798</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>31.2403973448484</c:v>
+                  <c:v>31.167257368033098</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>31.377542002917799</c:v>
+                  <c:v>31.4537187530957</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>31.983108569936501</c:v>
+                  <c:v>31.850230213056602</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>32.1231952640251</c:v>
+                  <c:v>32.561559058305399</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>32.8605289887944</c:v>
+                  <c:v>33.337599575531002</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>33.633519500570699</c:v>
+                  <c:v>33.567364604831099</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>34.233684244491798</c:v>
+                  <c:v>33.931796195919198</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>34.794110902431299</c:v>
+                  <c:v>34.531350447008499</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>34.900669142158002</c:v>
+                  <c:v>34.593126821481597</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>35.456577978827397</c:v>
+                  <c:v>85.328440627799097</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1490,199 +1450,186 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>10.960392745720499</c:v>
+                  <c:v>10.923314</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.461562002452155</c:v>
+                  <c:v>11.424652099999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.962731259183808</c:v>
+                  <c:v>11.925990199999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.463900515915464</c:v>
+                  <c:v>12.427328299999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.965069772647119</c:v>
+                  <c:v>12.928666399999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.466239029378775</c:v>
+                  <c:v>13.430004499999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.96740828611043</c:v>
+                  <c:v>13.931342600000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14.468577542842084</c:v>
+                  <c:v>14.432680699999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14.969746799573739</c:v>
+                  <c:v>14.9340188</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15.470916056305395</c:v>
+                  <c:v>15.435356899999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15.972085313037049</c:v>
+                  <c:v>15.936695</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16.473254569768706</c:v>
+                  <c:v>16.438033099999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16.97442382650036</c:v>
+                  <c:v>16.9393712</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>17.475593083232013</c:v>
+                  <c:v>17.440709300000002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>17.97676233996367</c:v>
+                  <c:v>17.9420474</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>18.477931596695324</c:v>
+                  <c:v>18.443385499999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>18.979100853426978</c:v>
+                  <c:v>18.9447236</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>19.480270110158635</c:v>
+                  <c:v>19.446061700000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>19.981439366890292</c:v>
+                  <c:v>19.947399799999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20.482608623621942</c:v>
+                  <c:v>20.448737899999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20.9837778803536</c:v>
+                  <c:v>20.950075999999999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21.484947137085257</c:v>
+                  <c:v>21.451414100000001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>21.986116393816907</c:v>
+                  <c:v>21.952752199999999</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>22.487285650548564</c:v>
+                  <c:v>22.454090299999997</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>22.988454907280222</c:v>
+                  <c:v>22.955428400000002</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>23.489624164011875</c:v>
+                  <c:v>23.456766500000001</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>23.990793420743529</c:v>
+                  <c:v>23.958104599999999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>24.491962677475186</c:v>
+                  <c:v>24.4594427</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>24.99313193420684</c:v>
+                  <c:v>24.960780800000002</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>25.494301190938494</c:v>
+                  <c:v>25.4621189</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>25.995470447670151</c:v>
+                  <c:v>25.963456999999998</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>26.496639704401804</c:v>
+                  <c:v>26.4647951</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>26.997808961133458</c:v>
+                  <c:v>26.966133200000002</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>27.498978217865115</c:v>
+                  <c:v>27.4674713</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>28.000147474596773</c:v>
+                  <c:v>27.968809399999998</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>28.501316731328423</c:v>
+                  <c:v>28.470147500000003</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>29.00248598806008</c:v>
+                  <c:v>28.971485600000001</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>29.503655244791737</c:v>
+                  <c:v>29.472823699999999</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>30.004824501523387</c:v>
+                  <c:v>29.974161799999997</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>30.505993758255045</c:v>
+                  <c:v>30.475499900000003</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>31.007163014986702</c:v>
+                  <c:v>30.976838000000001</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>31.508332271718352</c:v>
+                  <c:v>31.478176099999999</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>32.009501528450009</c:v>
+                  <c:v>31.979514199999997</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>32.510670785181667</c:v>
+                  <c:v>32.480852300000002</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>33.011840041913317</c:v>
+                  <c:v>32.9821904</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>33.513009298644974</c:v>
+                  <c:v>33.483528499999998</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>34.014178555376631</c:v>
+                  <c:v>33.984866599999997</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>34.515347812108288</c:v>
+                  <c:v>34.486204700000002</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>35.016517068839939</c:v>
+                  <c:v>34.9875428</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>35.517686325571596</c:v>
+                  <c:v>35.488880899999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="288419200"/>
-        <c:axId val="288419776"/>
+        <c:axId val="161363840"/>
+        <c:axId val="161365376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="288419200"/>
+        <c:axId val="161363840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="288419776"/>
+        <c:crossAx val="161365376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="288419776"/>
+        <c:axId val="161365376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="288419200"/>
+        <c:crossAx val="161363840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1690,15 +1637,13 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1738,81 +1683,49 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>10</xdr:col>
-          <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>30</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>12</xdr:col>
-          <xdr:colOff>371475</xdr:colOff>
-          <xdr:row>34</xdr:row>
-          <xdr:rowOff>152400</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2049" name="Object 1" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2049"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>485229</xdr:colOff>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>152238</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Рисунок 2"/>
+        <xdr:cNvPr id="2050" name="Picture 2"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="8915400" y="5734050"/>
-          <a:ext cx="4371429" cy="1295238"/>
+          <a:off x="9286875" y="5734050"/>
+          <a:ext cx="3857625" cy="1219200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1852,47 +1765,6 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>10</xdr:col>
-          <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>30</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>12</xdr:col>
-          <xdr:colOff>371475</xdr:colOff>
-          <xdr:row>34</xdr:row>
-          <xdr:rowOff>152400</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1025" name="Object 1" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1025"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
@@ -1901,32 +1773,41 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>609067</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>152237</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Рисунок 5"/>
+        <xdr:cNvPr id="1026" name="Picture 2"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="9305925" y="5724525"/>
-          <a:ext cx="4266667" cy="1304762"/>
+          <a:ext cx="3219450" cy="1285875"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -2009,7 +1890,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2044,7 +1924,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -2220,19 +2099,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:N51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+      <selection activeCell="X23" sqref="X23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4">
       <c r="B1" t="s">
         <v>6</v>
       </c>
@@ -2243,364 +2122,364 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4">
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1.8779868730901299</v>
+        <v>2.1872365302278198</v>
       </c>
       <c r="D2">
-        <f>B2*$H$35+$H$36</f>
-        <v>1.9729970999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" ref="D2:D33" si="0">B2*$H$35+$H$36</f>
+        <v>2.0357048</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4">
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1.04872358151307</v>
+        <v>0.76846818474802903</v>
       </c>
       <c r="D3">
-        <f>B3*$H$35+$H$36</f>
-        <v>0.97275376999999996</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>1.0347188</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4">
-        <v>0.11327510203060701</v>
+        <v>0.12998580019261799</v>
       </c>
       <c r="D4">
-        <f>B4*$H$35+$H$36</f>
-        <v>-2.7489560000000024E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>3.3732800000000118E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5">
-        <v>-0.970365400648735</v>
+        <v>-0.61072598466451999</v>
       </c>
       <c r="D5">
-        <f>B5*$H$35+$H$36</f>
-        <v>-1.02773289</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-0.96725319999999959</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
       <c r="B6">
         <v>4</v>
       </c>
       <c r="C6">
-        <v>-1.5357634841038601</v>
+        <v>-2.0551884125620599</v>
       </c>
       <c r="D6">
-        <f>B6*$H$35+$H$36</f>
-        <v>-2.0279762200000002</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-1.9682391999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
       <c r="B7">
         <v>5</v>
       </c>
       <c r="C7">
-        <v>-3.55584228067538</v>
+        <v>-3.2058232097278601</v>
       </c>
       <c r="D7">
-        <f>B7*$H$35+$H$36</f>
-        <v>-3.0282195500000002</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-2.9692251999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
       <c r="B8">
         <v>6</v>
       </c>
       <c r="C8">
-        <v>-3.9474333387310598</v>
+        <v>-3.6322381336357701</v>
       </c>
       <c r="D8">
-        <f>B8*$H$35+$H$36</f>
-        <v>-4.0284628800000002</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-3.9702111999999992</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
       <c r="B9">
         <v>7</v>
       </c>
       <c r="C9">
-        <v>-5.2650230324766403</v>
+        <v>-4.7736779123442004</v>
       </c>
       <c r="D9">
-        <f>B9*$H$35+$H$36</f>
-        <v>-5.0287062100000002</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-4.9711971999999989</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
       <c r="B10">
         <v>8</v>
       </c>
       <c r="C10">
-        <v>-5.6800610199923502</v>
+        <v>-6.0343239617040396</v>
       </c>
       <c r="D10">
-        <f>B10*$H$35+$H$36</f>
-        <v>-6.0289495400000002</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-5.9721831999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
       <c r="B11">
         <v>9</v>
       </c>
       <c r="C11">
-        <v>-7.1697105405861201</v>
+        <v>-6.8664907019936399</v>
       </c>
       <c r="D11">
-        <f>B11*$H$35+$H$36</f>
-        <v>-7.0291928700000001</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-6.9731691999999992</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
       <c r="B12">
         <v>10</v>
       </c>
       <c r="C12">
-        <v>-8.4510175509625007</v>
+        <v>-8.5173925622634901</v>
       </c>
       <c r="D12">
-        <f>B12*$H$35+$H$36</f>
-        <v>-8.0294361999999992</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-7.9741552000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
       <c r="B13">
         <v>11</v>
       </c>
       <c r="C13">
-        <v>-9.2922791804804898</v>
+        <v>-9.0479142547529108</v>
       </c>
       <c r="D13">
-        <f>B13*$H$35+$H$36</f>
-        <v>-9.0296795299999992</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-8.9751411999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
       <c r="B14">
         <v>12</v>
       </c>
       <c r="C14">
-        <v>-9.9736265496153393</v>
+        <v>-10.0479453771409</v>
       </c>
       <c r="D14">
-        <f>B14*$H$35+$H$36</f>
-        <v>-10.029922859999999</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-9.9761271999999988</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
       <c r="B15">
         <v>13</v>
       </c>
       <c r="C15">
-        <v>-11.554235043452</v>
+        <v>-10.850570603016999</v>
       </c>
       <c r="D15">
-        <f>B15*$H$35+$H$36</f>
-        <v>-11.030166189999999</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-10.9771132</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
       <c r="B16">
         <v>14</v>
       </c>
       <c r="C16">
-        <v>-12.1472185351737</v>
+        <v>-12.0362376775436</v>
       </c>
       <c r="D16">
-        <f>B16*$H$35+$H$36</f>
-        <v>-12.030409519999999</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-11.978099199999999</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14">
       <c r="B17">
         <v>15</v>
       </c>
       <c r="C17">
-        <v>-13.1447956249076</v>
+        <v>-12.7598399255463</v>
       </c>
       <c r="D17">
-        <f>B17*$H$35+$H$36</f>
-        <v>-13.030652849999999</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-12.9790852</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14">
       <c r="B18">
         <v>16</v>
       </c>
       <c r="C18">
-        <v>-13.7740670272578</v>
+        <v>-14.1339499801439</v>
       </c>
       <c r="D18">
-        <f>B18*$H$35+$H$36</f>
-        <v>-14.030896179999999</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-13.980071199999999</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14">
       <c r="B19">
         <v>17</v>
       </c>
       <c r="C19">
-        <v>-15.021928223002799</v>
+        <v>-14.705421269934799</v>
       </c>
       <c r="D19">
-        <f>B19*$H$35+$H$36</f>
-        <v>-15.031139509999999</v>
-      </c>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-14.9810572</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14">
       <c r="B20">
         <v>18</v>
       </c>
       <c r="C20">
-        <v>-15.9907308170609</v>
+        <v>-16.325043785474499</v>
       </c>
       <c r="D20">
-        <f>B20*$H$35+$H$36</f>
-        <v>-16.031382839999999</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-15.982043199999998</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14">
       <c r="B21">
         <v>19</v>
       </c>
       <c r="C21">
-        <v>-17.178151585884802</v>
+        <v>-17.149970099539999</v>
       </c>
       <c r="D21">
-        <f>B21*$H$35+$H$36</f>
-        <v>-17.031626169999999</v>
-      </c>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-16.983029199999997</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14">
       <c r="B22">
         <v>20</v>
       </c>
       <c r="C22">
-        <v>-18.6823021269769</v>
+        <v>-17.932165894331799</v>
       </c>
       <c r="D22">
-        <f>B22*$H$35+$H$36</f>
-        <v>-18.031869499999999</v>
-      </c>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-17.984015199999998</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14">
       <c r="B23">
         <v>21</v>
       </c>
       <c r="C23">
-        <v>-18.808398949611799</v>
+        <v>-19.0326634461819</v>
       </c>
       <c r="D23">
-        <f>B23*$H$35+$H$36</f>
-        <v>-19.032112829999999</v>
-      </c>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-18.985001199999996</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14">
       <c r="B24">
         <v>22</v>
       </c>
       <c r="C24">
-        <v>-19.669055903805202</v>
+        <v>-19.939167397070101</v>
       </c>
       <c r="D24">
-        <f>B24*$H$35+$H$36</f>
-        <v>-20.032356159999999</v>
-      </c>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-19.985987199999997</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14">
       <c r="B25">
         <v>23</v>
       </c>
       <c r="C25">
-        <v>-20.441670629015501</v>
+        <v>-20.779483445282001</v>
       </c>
       <c r="D25">
-        <f>B25*$H$35+$H$36</f>
-        <v>-21.032599489999999</v>
-      </c>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-20.986973199999998</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14">
       <c r="B26">
         <v>24</v>
       </c>
       <c r="C26">
-        <v>-22.079246939808399</v>
+        <v>-22.745912509466699</v>
       </c>
       <c r="D26">
-        <f>B26*$H$35+$H$36</f>
-        <v>-22.032842819999999</v>
-      </c>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-21.987959199999995</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14">
       <c r="B27">
         <v>25</v>
       </c>
       <c r="C27">
-        <v>-23.2016704762394</v>
+        <v>27.620864522782998</v>
       </c>
       <c r="D27">
-        <f>B27*$H$35+$H$36</f>
-        <v>-23.033086149999999</v>
-      </c>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-22.988945199999996</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14">
       <c r="B28">
         <v>26</v>
       </c>
       <c r="C28">
-        <v>-24.161095070809701</v>
+        <v>-23.7800308439706</v>
       </c>
       <c r="D28">
-        <f>B28*$H$35+$H$36</f>
-        <v>-24.033329479999999</v>
-      </c>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-23.989931199999997</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14">
       <c r="B29">
         <v>27</v>
       </c>
       <c r="C29">
-        <v>-24.8766582272454</v>
+        <v>-25.331097463237398</v>
       </c>
       <c r="D29">
-        <f>B29*$H$35+$H$36</f>
-        <v>-25.033572809999999</v>
-      </c>
-    </row>
-    <row r="30" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>-24.990917199999998</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" ht="15.75" thickBot="1">
       <c r="B30">
         <v>28</v>
       </c>
       <c r="C30">
-        <v>-26.0737989722431</v>
+        <v>-26.1627850994984</v>
       </c>
       <c r="D30">
-        <f>B30*$H$35+$H$36</f>
-        <v>-26.033816139999999</v>
-      </c>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-25.991903199999996</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14">
       <c r="B31">
         <v>29</v>
       </c>
       <c r="C31">
-        <v>-26.8424819664715</v>
+        <v>-26.734834108011</v>
       </c>
       <c r="D31">
-        <f>B31*$H$35+$H$36</f>
-        <v>-27.034059469999999</v>
+        <f t="shared" si="0"/>
+        <v>-26.992889199999997</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>0</v>
@@ -2614,16 +2493,16 @@
       <c r="M31" s="5"/>
       <c r="N31" s="6"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14">
       <c r="B32">
         <v>30</v>
       </c>
       <c r="C32">
-        <v>-27.646865616063</v>
+        <v>-28.003024083911299</v>
       </c>
       <c r="D32">
-        <f>B32*$H$35+$H$36</f>
-        <v>-28.034302799999999</v>
+        <f t="shared" si="0"/>
+        <v>-27.993875199999998</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>1</v>
@@ -2637,16 +2516,16 @@
       <c r="M32" s="8"/>
       <c r="N32" s="9"/>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14">
       <c r="B33">
         <v>31</v>
       </c>
       <c r="C33">
-        <v>-28.802772837058999</v>
+        <v>-28.810774424788701</v>
       </c>
       <c r="D33">
-        <f>B33*$H$35+$H$36</f>
-        <v>-29.034546129999999</v>
+        <f t="shared" si="0"/>
+        <v>-28.994861199999995</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>2</v>
@@ -2660,16 +2539,16 @@
       <c r="M33" s="8"/>
       <c r="N33" s="9"/>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14">
       <c r="B34">
         <v>32</v>
       </c>
       <c r="C34">
-        <v>-29.811864889133499</v>
+        <v>-30.255902003966298</v>
       </c>
       <c r="D34">
-        <f>B34*$H$35+$H$36</f>
-        <v>-30.034789459999999</v>
+        <f t="shared" ref="D34:D51" si="1">B34*$H$35+$H$36</f>
+        <v>-29.995847199999996</v>
       </c>
       <c r="G34" s="13"/>
       <c r="H34" s="13"/>
@@ -2679,22 +2558,22 @@
       <c r="M34" s="8"/>
       <c r="N34" s="9"/>
     </row>
-    <row r="35" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:14" ht="15.75" thickBot="1">
       <c r="B35">
         <v>33</v>
       </c>
       <c r="C35">
-        <v>-30.819992693750301</v>
+        <v>-30.796419406734699</v>
       </c>
       <c r="D35">
-        <f>B35*$H$35+$H$36</f>
-        <v>-31.035032790000002</v>
+        <f t="shared" si="1"/>
+        <v>-30.996833199999994</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H35" s="2">
-        <v>-1.00024333</v>
+        <v>-1.0009859999999999</v>
       </c>
       <c r="J35" s="10"/>
       <c r="K35" s="11"/>
@@ -2702,208 +2581,208 @@
       <c r="M35" s="11"/>
       <c r="N35" s="12"/>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:14">
       <c r="B36">
         <v>34</v>
       </c>
       <c r="C36">
-        <v>-32.047658828927297</v>
+        <v>-31.7479428462368</v>
       </c>
       <c r="D36">
-        <f>B36*$H$35+$H$36</f>
-        <v>-32.035276119999999</v>
+        <f t="shared" si="1"/>
+        <v>-31.997819199999999</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H36" s="1">
-        <v>1.9729970999999999</v>
-      </c>
-    </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+        <v>2.0357048</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14">
       <c r="B37">
         <v>35</v>
       </c>
       <c r="C37">
-        <v>-33.6739143451302</v>
+        <v>-32.715962063456402</v>
       </c>
       <c r="D37">
-        <f>B37*$H$35+$H$36</f>
-        <v>-33.035519449999995</v>
+        <f t="shared" si="1"/>
+        <v>-32.9988052</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>5</v>
       </c>
       <c r="H37" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14">
       <c r="B38">
         <v>36</v>
       </c>
       <c r="C38">
-        <v>-33.887727907480901</v>
+        <v>-33.788552156288702</v>
       </c>
       <c r="D38">
-        <f>B38*$H$35+$H$36</f>
-        <v>-34.035762779999999</v>
-      </c>
-    </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>-33.999791199999997</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14">
       <c r="B39">
         <v>37</v>
       </c>
       <c r="C39">
-        <v>-34.772603885398603</v>
+        <v>-35.3104929373755</v>
       </c>
       <c r="D39">
-        <f>B39*$H$35+$H$36</f>
-        <v>-35.036006110000002</v>
-      </c>
-    </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>-35.000777200000002</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14">
       <c r="B40">
         <v>38</v>
       </c>
       <c r="C40">
-        <v>-36.140216914653102</v>
+        <v>-35.793556789608402</v>
       </c>
       <c r="D40">
-        <f>B40*$H$35+$H$36</f>
-        <v>-36.036249439999999</v>
-      </c>
-    </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>-36.001763199999999</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14">
       <c r="B41">
         <v>39</v>
       </c>
       <c r="C41">
-        <v>-37.127676445117302</v>
+        <v>-37.551172608759998</v>
       </c>
       <c r="D41">
-        <f>B41*$H$35+$H$36</f>
-        <v>-37.036492769999995</v>
-      </c>
-    </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>-37.002749199999997</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14">
       <c r="B42">
         <v>40</v>
       </c>
       <c r="C42">
-        <v>-37.357523155733901</v>
+        <v>-38.233033222547199</v>
       </c>
       <c r="D42">
-        <f>B42*$H$35+$H$36</f>
-        <v>-38.036736099999999</v>
-      </c>
-    </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>-38.003735200000001</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14">
       <c r="B43">
         <v>41</v>
       </c>
       <c r="C43">
-        <v>-38.412719576328598</v>
+        <v>-39.0356740179909</v>
       </c>
       <c r="D43">
-        <f>B43*$H$35+$H$36</f>
-        <v>-39.036979430000002</v>
-      </c>
-    </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>-39.004721199999999</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14">
       <c r="B44">
         <v>42</v>
       </c>
       <c r="C44">
-        <v>-40.113887699237203</v>
+        <v>-40.3164542089959</v>
       </c>
       <c r="D44">
-        <f>B44*$H$35+$H$36</f>
-        <v>-40.037222759999999</v>
-      </c>
-    </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>-40.005707199999996</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14">
       <c r="B45">
         <v>43</v>
       </c>
       <c r="C45">
-        <v>-41.318860316085697</v>
+        <v>-41.412564372814401</v>
       </c>
       <c r="D45">
-        <f>B45*$H$35+$H$36</f>
-        <v>-41.037466089999995</v>
-      </c>
-    </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>-41.006693200000001</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14">
       <c r="B46">
         <v>44</v>
       </c>
       <c r="C46">
-        <v>-42.261308051520302</v>
+        <v>-41.805156520057999</v>
       </c>
       <c r="D46">
-        <f>B46*$H$35+$H$36</f>
-        <v>-42.037709419999999</v>
-      </c>
-    </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>-42.007679199999998</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14">
       <c r="B47">
         <v>45</v>
       </c>
       <c r="C47">
-        <v>-43.136103750477503</v>
+        <v>-42.836516776315001</v>
       </c>
       <c r="D47">
-        <f>B47*$H$35+$H$36</f>
-        <v>-43.037952750000002</v>
-      </c>
-    </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>-43.008665199999996</v>
+      </c>
+    </row>
+    <row r="48" spans="2:14">
       <c r="B48">
         <v>46</v>
       </c>
       <c r="C48">
-        <v>-44.212076715397799</v>
+        <v>-44.089090134612803</v>
       </c>
       <c r="D48">
-        <f>B48*$H$35+$H$36</f>
-        <v>-44.038196079999999</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>-44.0096512</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4">
       <c r="B49">
         <v>47</v>
       </c>
       <c r="C49">
-        <v>-45.061877624970499</v>
+        <v>-44.694716291171602</v>
       </c>
       <c r="D49">
-        <f>B49*$H$35+$H$36</f>
-        <v>-45.038439409999995</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>-45.010637199999998</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4">
       <c r="B50">
         <v>48</v>
       </c>
       <c r="C50">
-        <v>-46.283588040614902</v>
+        <v>-45.795324866667102</v>
       </c>
       <c r="D50">
-        <f>B50*$H$35+$H$36</f>
-        <v>-46.038682739999999</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>-46.011623199999995</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4">
       <c r="B51">
         <v>49</v>
       </c>
       <c r="C51">
-        <v>-47.205619537623299</v>
+        <v>2.81341692842153</v>
       </c>
       <c r="D51">
-        <f>B51*$H$35+$H$36</f>
-        <v>-47.038926070000002</v>
+        <f t="shared" si="1"/>
+        <v>-47.0126092</v>
       </c>
     </row>
   </sheetData>
@@ -2915,49 +2794,26 @@
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <oleObjects>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <oleObject progId="Equation.3" shapeId="2049" r:id="rId3">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId4">
-            <anchor moveWithCells="1" sizeWithCells="1">
-              <from>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>76200</xdr:colOff>
-                <xdr:row>30</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>12</xdr:col>
-                <xdr:colOff>371475</xdr:colOff>
-                <xdr:row>34</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </to>
-            </anchor>
-          </objectPr>
-        </oleObject>
-      </mc:Choice>
-      <mc:Fallback>
-        <oleObject progId="Equation.3" shapeId="2049" r:id="rId3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
+    <oleObject progId="Equation.3" shapeId="2049" r:id="rId3"/>
   </oleObjects>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="AA16" sqref="AA16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4">
       <c r="B1" t="s">
         <v>6</v>
       </c>
@@ -2968,364 +2824,364 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4">
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>11.0476492914418</v>
+        <v>10.804663868816901</v>
       </c>
       <c r="D2">
-        <f>B2*$H$35+$H$36</f>
-        <v>10.960392745720499</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" ref="D2:D33" si="0">B2*$H$35+$H$36</f>
+        <v>10.923314</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4">
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>11.2545142953972</v>
+        <v>11.4045971550992</v>
       </c>
       <c r="D3">
-        <f>B3*$H$35+$H$36</f>
-        <v>11.461562002452155</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>11.424652099999999</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4">
-        <v>12.0478921072727</v>
+        <v>12.313315363637299</v>
       </c>
       <c r="D4">
-        <f>B4*$H$35+$H$36</f>
-        <v>11.962731259183808</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>11.925990199999999</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5">
-        <v>12.6540812020831</v>
+        <v>12.184555948423499</v>
       </c>
       <c r="D5">
-        <f>B5*$H$35+$H$36</f>
-        <v>12.463900515915464</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>12.427328299999999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
       <c r="B6">
         <v>4</v>
       </c>
       <c r="C6">
-        <v>12.890539310361</v>
+        <v>12.7327705178178</v>
       </c>
       <c r="D6">
-        <f>B6*$H$35+$H$36</f>
-        <v>12.965069772647119</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>12.928666399999999</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
       <c r="B7">
         <v>5</v>
       </c>
       <c r="C7">
-        <v>13.0601016876484</v>
+        <v>13.389541335015201</v>
       </c>
       <c r="D7">
-        <f>B7*$H$35+$H$36</f>
-        <v>13.466239029378775</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>13.430004499999999</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
       <c r="B8">
         <v>6</v>
       </c>
       <c r="C8">
-        <v>13.8883663155998</v>
+        <v>13.7616845144299</v>
       </c>
       <c r="D8">
-        <f>B8*$H$35+$H$36</f>
-        <v>13.96740828611043</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>13.931342600000001</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
       <c r="B9">
         <v>7</v>
       </c>
       <c r="C9">
-        <v>14.352919110137501</v>
+        <v>14.6842531129822</v>
       </c>
       <c r="D9">
-        <f>B9*$H$35+$H$36</f>
-        <v>14.468577542842084</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>14.432680699999999</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
       <c r="B10">
         <v>8</v>
       </c>
       <c r="C10">
-        <v>15.023211056700401</v>
+        <v>15.114017126027999</v>
       </c>
       <c r="D10">
-        <f>B10*$H$35+$H$36</f>
-        <v>14.969746799573739</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>14.9340188</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
       <c r="B11">
         <v>9</v>
       </c>
       <c r="C11">
-        <v>15.5941525930727</v>
+        <v>15.3782795925491</v>
       </c>
       <c r="D11">
-        <f>B11*$H$35+$H$36</f>
-        <v>15.470916056305395</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>15.435356899999999</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
       <c r="B12">
         <v>10</v>
       </c>
       <c r="C12">
-        <v>15.984676567108201</v>
+        <v>16.381627265468101</v>
       </c>
       <c r="D12">
-        <f>B12*$H$35+$H$36</f>
-        <v>15.972085313037049</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>15.936695</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
       <c r="B13">
         <v>11</v>
       </c>
       <c r="C13">
-        <v>16.990543270915001</v>
+        <v>16.3852456138709</v>
       </c>
       <c r="D13">
-        <f>B13*$H$35+$H$36</f>
-        <v>16.473254569768706</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>16.438033099999998</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
       <c r="B14">
         <v>12</v>
       </c>
       <c r="C14">
-        <v>17.401500291947201</v>
+        <v>17.070852956278099</v>
       </c>
       <c r="D14">
-        <f>B14*$H$35+$H$36</f>
-        <v>16.97442382650036</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>16.9393712</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
       <c r="B15">
         <v>13</v>
       </c>
       <c r="C15">
-        <v>17.5194324450365</v>
+        <v>16.898206296146999</v>
       </c>
       <c r="D15">
-        <f>B15*$H$35+$H$36</f>
-        <v>17.475593083232013</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>17.440709300000002</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
       <c r="B16">
         <v>14</v>
       </c>
       <c r="C16">
-        <v>18.3529038861057</v>
+        <v>17.738664734695401</v>
       </c>
       <c r="D16">
-        <f>B16*$H$35+$H$36</f>
-        <v>17.97676233996367</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>17.9420474</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14">
       <c r="B17">
         <v>15</v>
       </c>
       <c r="C17">
-        <v>18.660639069482599</v>
+        <v>18.675725948944301</v>
       </c>
       <c r="D17">
-        <f>B17*$H$35+$H$36</f>
-        <v>18.477931596695324</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>18.443385499999998</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14">
       <c r="B18">
         <v>16</v>
       </c>
       <c r="C18">
-        <v>18.6534590387535</v>
+        <v>19.291096258252701</v>
       </c>
       <c r="D18">
-        <f>B18*$H$35+$H$36</f>
-        <v>18.979100853426978</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>18.9447236</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14">
       <c r="B19">
         <v>17</v>
       </c>
       <c r="C19">
-        <v>19.520696531085001</v>
+        <v>19.6516583360029</v>
       </c>
       <c r="D19">
-        <f>B19*$H$35+$H$36</f>
-        <v>19.480270110158635</v>
-      </c>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>19.446061700000001</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14">
       <c r="B20">
         <v>18</v>
       </c>
       <c r="C20">
-        <v>20.257854904623802</v>
+        <v>20.069991577437701</v>
       </c>
       <c r="D20">
-        <f>B20*$H$35+$H$36</f>
-        <v>19.981439366890292</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>19.947399799999999</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14">
       <c r="B21">
         <v>19</v>
       </c>
       <c r="C21">
-        <v>20.506458991237299</v>
+        <v>20.527395543142202</v>
       </c>
       <c r="D21">
-        <f>B21*$H$35+$H$36</f>
-        <v>20.482608623621942</v>
-      </c>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>20.448737899999998</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14">
       <c r="B22">
         <v>20</v>
       </c>
       <c r="C22">
-        <v>21.2606427062012</v>
+        <v>20.8450971527189</v>
       </c>
       <c r="D22">
-        <f>B22*$H$35+$H$36</f>
-        <v>20.9837778803536</v>
-      </c>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>20.950075999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14">
       <c r="B23">
         <v>21</v>
       </c>
       <c r="C23">
-        <v>21.598616288808199</v>
+        <v>21.541101164524498</v>
       </c>
       <c r="D23">
-        <f>B23*$H$35+$H$36</f>
-        <v>21.484947137085257</v>
-      </c>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>21.451414100000001</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14">
       <c r="B24">
         <v>22</v>
       </c>
       <c r="C24">
-        <v>21.942345412099101</v>
+        <v>21.866320369385001</v>
       </c>
       <c r="D24">
-        <f>B24*$H$35+$H$36</f>
-        <v>21.986116393816907</v>
-      </c>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>21.952752199999999</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14">
       <c r="B25">
         <v>23</v>
       </c>
       <c r="C25">
-        <v>22.496036689624599</v>
+        <v>22.355525151997401</v>
       </c>
       <c r="D25">
-        <f>B25*$H$35+$H$36</f>
-        <v>22.487285650548564</v>
-      </c>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>22.454090299999997</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14">
       <c r="B26">
         <v>24</v>
       </c>
       <c r="C26">
-        <v>22.686528292361</v>
+        <v>22.848657320085199</v>
       </c>
       <c r="D26">
-        <f>B26*$H$35+$H$36</f>
-        <v>22.988454907280222</v>
-      </c>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>22.955428400000002</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14">
       <c r="B27">
         <v>25</v>
       </c>
       <c r="C27">
-        <v>23.852812302278299</v>
+        <v>-26.525142054605301</v>
       </c>
       <c r="D27">
-        <f>B27*$H$35+$H$36</f>
-        <v>23.489624164011875</v>
-      </c>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>23.456766500000001</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14">
       <c r="B28">
         <v>26</v>
       </c>
       <c r="C28">
-        <v>23.694499773141999</v>
+        <v>23.615863345663801</v>
       </c>
       <c r="D28">
-        <f>B28*$H$35+$H$36</f>
-        <v>23.990793420743529</v>
-      </c>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>23.958104599999999</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14">
       <c r="B29">
         <v>27</v>
       </c>
       <c r="C29">
-        <v>24.7768002538944</v>
+        <v>24.231967601597901</v>
       </c>
       <c r="D29">
-        <f>B29*$H$35+$H$36</f>
-        <v>24.491962677475186</v>
-      </c>
-    </row>
-    <row r="30" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>24.4594427</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" ht="15.75" thickBot="1">
       <c r="B30">
         <v>28</v>
       </c>
       <c r="C30">
-        <v>24.654619350632998</v>
+        <v>25.1513006226442</v>
       </c>
       <c r="D30">
-        <f>B30*$H$35+$H$36</f>
-        <v>24.99313193420684</v>
-      </c>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>24.960780800000002</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14">
       <c r="B31">
         <v>29</v>
       </c>
       <c r="C31">
-        <v>25.4495145582415</v>
+        <v>25.1571646801257</v>
       </c>
       <c r="D31">
-        <f>B31*$H$35+$H$36</f>
-        <v>25.494301190938494</v>
+        <f t="shared" si="0"/>
+        <v>25.4621189</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>0</v>
@@ -3339,16 +3195,16 @@
       <c r="M31" s="5"/>
       <c r="N31" s="6"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14">
       <c r="B32">
         <v>30</v>
       </c>
       <c r="C32">
-        <v>25.671706507480401</v>
+        <v>25.777402875439702</v>
       </c>
       <c r="D32">
-        <f>B32*$H$35+$H$36</f>
-        <v>25.995470447670151</v>
+        <f t="shared" si="0"/>
+        <v>25.963456999999998</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>1</v>
@@ -3362,16 +3218,16 @@
       <c r="M32" s="8"/>
       <c r="N32" s="9"/>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14">
       <c r="B33">
         <v>31</v>
       </c>
       <c r="C33">
-        <v>26.440430508471</v>
+        <v>26.264182636778699</v>
       </c>
       <c r="D33">
-        <f>B33*$H$35+$H$36</f>
-        <v>26.496639704401804</v>
+        <f t="shared" si="0"/>
+        <v>26.4647951</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>2</v>
@@ -3385,16 +3241,16 @@
       <c r="M33" s="8"/>
       <c r="N33" s="9"/>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14">
       <c r="B34">
         <v>32</v>
       </c>
       <c r="C34">
-        <v>26.939591096962101</v>
+        <v>26.884713652702501</v>
       </c>
       <c r="D34">
-        <f>B34*$H$35+$H$36</f>
-        <v>26.997808961133458</v>
+        <f t="shared" ref="D34:D51" si="1">B34*$H$35+$H$36</f>
+        <v>26.966133200000002</v>
       </c>
       <c r="G34" s="13"/>
       <c r="H34" s="13"/>
@@ -3404,22 +3260,22 @@
       <c r="M34" s="8"/>
       <c r="N34" s="9"/>
     </row>
-    <row r="35" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:14" ht="15.75" thickBot="1">
       <c r="B35">
         <v>33</v>
       </c>
       <c r="C35">
-        <v>27.662355371868099</v>
+        <v>27.110427364873299</v>
       </c>
       <c r="D35">
-        <f>B35*$H$35+$H$36</f>
-        <v>27.498978217865115</v>
+        <f t="shared" si="1"/>
+        <v>27.4674713</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H35" s="2">
-        <v>0.50116925673165502</v>
+        <v>0.50133810000000001</v>
       </c>
       <c r="J35" s="10"/>
       <c r="K35" s="11"/>
@@ -3427,34 +3283,34 @@
       <c r="M35" s="11"/>
       <c r="N35" s="12"/>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:14">
       <c r="B36">
         <v>34</v>
       </c>
       <c r="C36">
-        <v>27.7275294876614</v>
+        <v>28.432701226955999</v>
       </c>
       <c r="D36">
-        <f>B36*$H$35+$H$36</f>
-        <v>28.000147474596773</v>
+        <f t="shared" si="1"/>
+        <v>27.968809399999998</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H36" s="1">
-        <v>10.960392745720499</v>
-      </c>
-    </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+        <v>10.923314</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14">
       <c r="B37">
         <v>35</v>
       </c>
       <c r="C37">
-        <v>28.2897176785849</v>
+        <v>28.544306139202899</v>
       </c>
       <c r="D37">
-        <f>B37*$H$35+$H$36</f>
-        <v>28.501316731328423</v>
+        <f t="shared" si="1"/>
+        <v>28.470147500000003</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>5</v>
@@ -3463,172 +3319,172 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:14">
       <c r="B38">
         <v>36</v>
       </c>
       <c r="C38">
-        <v>29.012454496925098</v>
+        <v>29.160002278887799</v>
       </c>
       <c r="D38">
-        <f>B38*$H$35+$H$36</f>
-        <v>29.00248598806008</v>
-      </c>
-    </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>28.971485600000001</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14">
       <c r="B39">
         <v>37</v>
       </c>
       <c r="C39">
-        <v>29.658489995003102</v>
+        <v>29.578328888553099</v>
       </c>
       <c r="D39">
-        <f>B39*$H$35+$H$36</f>
-        <v>29.503655244791737</v>
-      </c>
-    </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>29.472823699999999</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14">
       <c r="B40">
         <v>38</v>
       </c>
       <c r="C40">
-        <v>30.185380841339601</v>
+        <v>29.926789950360298</v>
       </c>
       <c r="D40">
-        <f>B40*$H$35+$H$36</f>
-        <v>30.004824501523387</v>
-      </c>
-    </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>29.974161799999997</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14">
       <c r="B41">
         <v>39</v>
       </c>
       <c r="C41">
-        <v>30.475054220399802</v>
+        <v>30.624062254067798</v>
       </c>
       <c r="D41">
-        <f>B41*$H$35+$H$36</f>
-        <v>30.505993758255045</v>
-      </c>
-    </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>30.475499900000003</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14">
       <c r="B42">
         <v>40</v>
       </c>
       <c r="C42">
-        <v>31.2403973448484</v>
+        <v>31.167257368033098</v>
       </c>
       <c r="D42">
-        <f>B42*$H$35+$H$36</f>
-        <v>31.007163014986702</v>
-      </c>
-    </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>30.976838000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14">
       <c r="B43">
         <v>41</v>
       </c>
       <c r="C43">
-        <v>31.377542002917799</v>
+        <v>31.4537187530957</v>
       </c>
       <c r="D43">
-        <f>B43*$H$35+$H$36</f>
-        <v>31.508332271718352</v>
-      </c>
-    </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>31.478176099999999</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14">
       <c r="B44">
         <v>42</v>
       </c>
       <c r="C44">
-        <v>31.983108569936501</v>
+        <v>31.850230213056602</v>
       </c>
       <c r="D44">
-        <f>B44*$H$35+$H$36</f>
-        <v>32.009501528450009</v>
-      </c>
-    </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>31.979514199999997</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14">
       <c r="B45">
         <v>43</v>
       </c>
       <c r="C45">
-        <v>32.1231952640251</v>
+        <v>32.561559058305399</v>
       </c>
       <c r="D45">
-        <f>B45*$H$35+$H$36</f>
-        <v>32.510670785181667</v>
-      </c>
-    </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>32.480852300000002</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14">
       <c r="B46">
         <v>44</v>
       </c>
       <c r="C46">
-        <v>32.8605289887944</v>
+        <v>33.337599575531002</v>
       </c>
       <c r="D46">
-        <f>B46*$H$35+$H$36</f>
-        <v>33.011840041913317</v>
-      </c>
-    </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>32.9821904</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14">
       <c r="B47">
         <v>45</v>
       </c>
       <c r="C47">
-        <v>33.633519500570699</v>
+        <v>33.567364604831099</v>
       </c>
       <c r="D47">
-        <f>B47*$H$35+$H$36</f>
-        <v>33.513009298644974</v>
-      </c>
-    </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>33.483528499999998</v>
+      </c>
+    </row>
+    <row r="48" spans="2:14">
       <c r="B48">
         <v>46</v>
       </c>
       <c r="C48">
-        <v>34.233684244491798</v>
+        <v>33.931796195919198</v>
       </c>
       <c r="D48">
-        <f>B48*$H$35+$H$36</f>
-        <v>34.014178555376631</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>33.984866599999997</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4">
       <c r="B49">
         <v>47</v>
       </c>
       <c r="C49">
-        <v>34.794110902431299</v>
+        <v>34.531350447008499</v>
       </c>
       <c r="D49">
-        <f>B49*$H$35+$H$36</f>
-        <v>34.515347812108288</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>34.486204700000002</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4">
       <c r="B50">
         <v>48</v>
       </c>
       <c r="C50">
-        <v>34.900669142158002</v>
+        <v>34.593126821481597</v>
       </c>
       <c r="D50">
-        <f>B50*$H$35+$H$36</f>
-        <v>35.016517068839939</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>34.9875428</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4">
       <c r="B51">
         <v>49</v>
       </c>
       <c r="C51">
-        <v>35.456577978827397</v>
+        <v>85.328440627799097</v>
       </c>
       <c r="D51">
-        <f>B51*$H$35+$H$36</f>
-        <v>35.517686325571596</v>
+        <f t="shared" si="1"/>
+        <v>35.488880899999998</v>
       </c>
     </row>
   </sheetData>
@@ -3640,43 +3496,7 @@
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <oleObjects>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <oleObject progId="Equation.3" shapeId="1025" r:id="rId3">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId4">
-            <anchor moveWithCells="1" sizeWithCells="1">
-              <from>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>76200</xdr:colOff>
-                <xdr:row>30</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>12</xdr:col>
-                <xdr:colOff>371475</xdr:colOff>
-                <xdr:row>34</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </to>
-            </anchor>
-          </objectPr>
-        </oleObject>
-      </mc:Choice>
-      <mc:Fallback>
-        <oleObject progId="Equation.3" shapeId="1025" r:id="rId3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
+    <oleObject progId="Equation.3" shapeId="1025" r:id="rId3"/>
   </oleObjects>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>